<commit_message>
includes expected ranges from Price et al 2015
</commit_message>
<xml_diff>
--- a/LH_Invariants_w_expected_range.xlsx
+++ b/LH_Invariants_w_expected_range.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="LH_Invariants_w_expected_range." sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -182,16 +182,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -338,23 +331,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -681,7 +674,7 @@
       <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="18" t="s">
+      <c r="N1" s="17" t="s">
         <v>22</v>
       </c>
       <c r="O1" s="2" t="s">
@@ -690,13 +683,13 @@
       <c r="P1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="R1" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
       <c r="W1" s="4"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -733,33 +726,33 @@
       <c r="K2">
         <v>3.5329999999999999</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="12">
         <v>1.375</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <v>0.57808667211774301</v>
       </c>
-      <c r="N2" s="14">
+      <c r="N2" s="13">
         <v>0.68571428571428605</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="13">
         <f>M2-N2</f>
         <v>-0.10762761359654305</v>
       </c>
       <c r="P2" s="5">
         <v>2.97</v>
       </c>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12" t="s">
+      <c r="R2" s="11"/>
+      <c r="S2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="12" t="s">
+      <c r="T2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="12" t="s">
+      <c r="V2" s="11" t="s">
         <v>23</v>
       </c>
       <c r="W2" s="4"/>
@@ -798,16 +791,16 @@
       <c r="K3">
         <v>2.4649329999999998</v>
       </c>
-      <c r="L3" s="13">
+      <c r="L3" s="12">
         <v>0.38775510204081598</v>
       </c>
-      <c r="M3" s="14">
+      <c r="M3" s="13">
         <v>0.60606060606060597</v>
       </c>
-      <c r="N3" s="14">
+      <c r="N3" s="13">
         <v>0.88554216867469904</v>
       </c>
-      <c r="O3" s="14">
+      <c r="O3" s="13">
         <f t="shared" ref="O3:O11" si="0">M3-N3</f>
         <v>-0.27948156261409307</v>
       </c>
@@ -865,16 +858,16 @@
       <c r="K4">
         <v>2.75</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="12">
         <v>1.43333333333333</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="13">
         <v>0.569608078865112</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="13">
         <v>0.67669172932330801</v>
       </c>
-      <c r="O4" s="14">
+      <c r="O4" s="13">
         <f t="shared" si="0"/>
         <v>-0.10708365045819601</v>
       </c>
@@ -931,16 +924,16 @@
       <c r="K5">
         <v>2.3645700000000001</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="12">
         <v>1.04892647058824</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="13">
         <v>0.55769824281945302</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="13">
         <v>0.74093714020056201</v>
       </c>
-      <c r="O5" s="14">
+      <c r="O5" s="13">
         <f t="shared" si="0"/>
         <v>-0.18323889738110899</v>
       </c>
@@ -997,16 +990,16 @@
       <c r="K6">
         <v>2.7189999999999999</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="16">
         <v>3.08838144329897</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <v>0.55090759195109495</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <v>0.492741794833154</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <f t="shared" si="0"/>
         <v>5.8165797117940954E-2</v>
       </c>
@@ -1063,16 +1056,16 @@
       <c r="K7">
         <v>3</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="12">
         <v>0.90945120740740704</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="13">
         <v>0.62627482501648701</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="13">
         <v>0.76737113237678201</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O7" s="13">
         <f t="shared" si="0"/>
         <v>-0.14109630736029499</v>
       </c>
@@ -1117,16 +1110,16 @@
       <c r="K8">
         <v>2.7812000000000001</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>3.32859142</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="13">
         <v>0.44266857756176597</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="13">
         <v>0.47403913460414199</v>
       </c>
-      <c r="O8" s="14">
+      <c r="O8" s="13">
         <f t="shared" si="0"/>
         <v>-3.1370557042376013E-2</v>
       </c>
@@ -1171,16 +1164,16 @@
       <c r="K9">
         <v>3</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="12">
         <v>0.60276303239436602</v>
       </c>
-      <c r="M9" s="19">
+      <c r="M9" s="18">
         <v>0.92723164556962001</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="13">
         <v>0.83269423301654799</v>
       </c>
-      <c r="O9" s="14">
+      <c r="O9" s="13">
         <f t="shared" si="0"/>
         <v>9.453741255307202E-2</v>
       </c>
@@ -1225,16 +1218,16 @@
       <c r="K10">
         <v>3</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="12">
         <v>1.1000000000000001</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="13">
         <v>0.63840123660477399</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="13">
         <v>0.73170731707317105</v>
       </c>
-      <c r="O10" s="14">
+      <c r="O10" s="13">
         <f t="shared" si="0"/>
         <v>-9.3306080468397057E-2</v>
       </c>
@@ -1279,20 +1272,20 @@
       <c r="K11">
         <v>3.0411999999999999</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="15">
         <v>4.7777777777777803</v>
       </c>
-      <c r="M11" s="15">
+      <c r="M11" s="14">
         <v>0.55396199354607401</v>
       </c>
-      <c r="N11" s="15">
+      <c r="N11" s="14">
         <v>0.38571428571428601</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <f t="shared" si="0"/>
         <v>0.168247707831788</v>
       </c>
-      <c r="P11" s="20">
+      <c r="P11" s="19">
         <v>7.5250000000000004</v>
       </c>
     </row>

</xml_diff>